<commit_message>
Organizando el diagrama de gantt
</commit_message>
<xml_diff>
--- a/proyecto/Diagrama Gantt_Pañales Santiago.xlsx
+++ b/proyecto/Diagrama Gantt_Pañales Santiago.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\WSTAR\Desktop\Pa-alera-Santiago\proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mateo\Desktop\Pa-alera-Santiago\proyecto\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA4C79C1-EF3F-44B0-BFE2-DB536F455BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="9045" tabRatio="432"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="26">
   <si>
     <t>Actividades</t>
   </si>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -139,7 +140,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -158,8 +159,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -182,22 +195,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -219,19 +221,66 @@
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="4">
+    <dxf>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="9" tint="0.40000610370189521"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <gradientFill degree="45">
+          <stop position="0">
+            <color theme="0"/>
+          </stop>
+          <stop position="1">
+            <color theme="5"/>
+          </stop>
+        </gradientFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <gradientFill degree="45">
@@ -258,6 +307,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9966"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -531,20 +585,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr autoPageBreaks="0"/>
   </sheetPr>
-  <dimension ref="A4:AF25"/>
+  <dimension ref="A4:AI25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="AK19" sqref="AK19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
     <col min="6" max="6" width="4.42578125" customWidth="1"/>
     <col min="7" max="12" width="5.28515625" customWidth="1"/>
@@ -566,9 +620,12 @@
     <col min="29" max="29" width="4.28515625" customWidth="1"/>
     <col min="30" max="31" width="4.140625" customWidth="1"/>
     <col min="32" max="32" width="4" customWidth="1"/>
+    <col min="33" max="33" width="6.7109375" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" customWidth="1"/>
+    <col min="35" max="35" width="5.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:32" ht="54.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" ht="54.75" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -665,172 +722,217 @@
       <c r="AF4" s="7">
         <v>44347</v>
       </c>
-    </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AG4" s="7">
+        <v>44362</v>
+      </c>
+      <c r="AH4" s="7">
+        <v>44370</v>
+      </c>
+      <c r="AI4" s="7">
+        <v>44377</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="8"/>
-      <c r="C5" s="9">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="11">
         <v>44328</v>
       </c>
-      <c r="D5" s="1"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="7"/>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7"/>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="7"/>
-      <c r="Z5" s="7"/>
-      <c r="AA5" s="7"/>
-      <c r="AB5" s="7"/>
-      <c r="AC5" s="7"/>
-      <c r="AD5" s="7"/>
-      <c r="AE5" s="7"/>
-      <c r="AF5" s="7"/>
-    </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D5" s="14">
+        <v>44347</v>
+      </c>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="16"/>
+      <c r="O5" s="16"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="16"/>
+      <c r="R5" s="16"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="16"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="16"/>
+      <c r="W5" s="16"/>
+      <c r="X5" s="16"/>
+      <c r="Y5" s="16"/>
+      <c r="Z5" s="16"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="16"/>
+      <c r="AD5" s="16"/>
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="2"/>
+      <c r="AH5" s="2"/>
+      <c r="AI5" s="2"/>
+    </row>
+    <row r="6" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-      <c r="K6" s="7"/>
-      <c r="L6" s="7"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="7"/>
-      <c r="O6" s="7"/>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="7"/>
-      <c r="Z6" s="7"/>
-      <c r="AA6" s="7"/>
-      <c r="AB6" s="7"/>
-      <c r="AC6" s="7"/>
-      <c r="AD6" s="7"/>
-      <c r="AE6" s="7"/>
-      <c r="AF6" s="7"/>
-    </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" s="14">
+        <v>44330</v>
+      </c>
+      <c r="D6" s="14">
+        <v>44330</v>
+      </c>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+      <c r="X6" s="15"/>
+      <c r="Y6" s="15"/>
+      <c r="Z6" s="15"/>
+      <c r="AA6" s="15"/>
+      <c r="AB6" s="15"/>
+      <c r="AC6" s="15"/>
+      <c r="AD6" s="15"/>
+      <c r="AE6" s="15"/>
+      <c r="AF6" s="15"/>
+      <c r="AG6" s="2"/>
+      <c r="AH6" s="2"/>
+      <c r="AI6" s="2"/>
+    </row>
+    <row r="7" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-      <c r="M7" s="7"/>
-      <c r="N7" s="7"/>
-      <c r="O7" s="7"/>
-      <c r="P7" s="7"/>
-      <c r="Q7" s="7"/>
-      <c r="R7" s="7"/>
-      <c r="S7" s="7"/>
-      <c r="T7" s="7"/>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="7"/>
-      <c r="Z7" s="7"/>
-      <c r="AA7" s="7"/>
-      <c r="AB7" s="7"/>
-      <c r="AC7" s="7"/>
-      <c r="AD7" s="7"/>
-      <c r="AE7" s="7"/>
-      <c r="AF7" s="7"/>
-    </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="14">
+        <v>44328</v>
+      </c>
+      <c r="D7" s="14">
+        <v>44342</v>
+      </c>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="16"/>
+      <c r="O7" s="16"/>
+      <c r="P7" s="16"/>
+      <c r="Q7" s="16"/>
+      <c r="R7" s="16"/>
+      <c r="S7" s="16"/>
+      <c r="T7" s="16"/>
+      <c r="U7" s="16"/>
+      <c r="V7" s="16"/>
+      <c r="W7" s="16"/>
+      <c r="X7" s="16"/>
+      <c r="Y7" s="16"/>
+      <c r="Z7" s="16"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="15"/>
+      <c r="AC7" s="15"/>
+      <c r="AD7" s="15"/>
+      <c r="AE7" s="15"/>
+      <c r="AF7" s="15"/>
+      <c r="AG7" s="2"/>
+      <c r="AH7" s="2"/>
+      <c r="AI7" s="2"/>
+    </row>
+    <row r="8" spans="1:35" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
-      <c r="K8" s="7"/>
-      <c r="L8" s="7"/>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="7"/>
-      <c r="Z8" s="7"/>
-      <c r="AA8" s="7"/>
-      <c r="AB8" s="7"/>
-      <c r="AC8" s="7"/>
-      <c r="AD8" s="7"/>
-      <c r="AE8" s="7"/>
-      <c r="AF8" s="7"/>
-    </row>
-    <row r="9" spans="1:32" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="14">
+        <v>44328</v>
+      </c>
+      <c r="D8" s="14">
+        <v>44335</v>
+      </c>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="16"/>
+      <c r="S8" s="16"/>
+      <c r="T8" s="16"/>
+      <c r="U8" s="15"/>
+      <c r="V8" s="15"/>
+      <c r="W8" s="15"/>
+      <c r="X8" s="15"/>
+      <c r="Y8" s="15"/>
+      <c r="Z8" s="15"/>
+      <c r="AA8" s="15"/>
+      <c r="AB8" s="15"/>
+      <c r="AC8" s="15"/>
+      <c r="AD8" s="15"/>
+      <c r="AE8" s="15"/>
+      <c r="AF8" s="15"/>
+      <c r="AG8" s="2"/>
+      <c r="AH8" s="2"/>
+      <c r="AI8" s="2"/>
+    </row>
+    <row r="9" spans="1:35" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="4"/>
-      <c r="C9" s="5">
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" s="10">
         <v>44320</v>
       </c>
-      <c r="D9" s="5">
+      <c r="D9" s="10">
         <v>44327</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
       <c r="M9" s="6"/>
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
@@ -851,12 +953,17 @@
       <c r="AD9" s="6"/>
       <c r="AE9" s="6"/>
       <c r="AF9" s="6"/>
-    </row>
-    <row r="10" spans="1:32" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG9" s="2"/>
+      <c r="AH9" s="2"/>
+      <c r="AI9" s="2"/>
+    </row>
+    <row r="10" spans="1:35" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="4"/>
+      <c r="B10" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="C10" s="5">
         <v>44328</v>
       </c>
@@ -871,32 +978,37 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
-      <c r="AA10" s="2"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="18"/>
+      <c r="O10" s="18"/>
+      <c r="P10" s="18"/>
+      <c r="Q10" s="18"/>
+      <c r="R10" s="18"/>
+      <c r="S10" s="18"/>
+      <c r="T10" s="18"/>
+      <c r="U10" s="18"/>
+      <c r="V10" s="18"/>
+      <c r="W10" s="18"/>
+      <c r="X10" s="18"/>
+      <c r="Y10" s="18"/>
+      <c r="Z10" s="18"/>
+      <c r="AA10" s="18"/>
       <c r="AB10" s="2"/>
       <c r="AC10" s="2"/>
       <c r="AD10" s="2"/>
       <c r="AE10" s="2"/>
       <c r="AF10" s="2"/>
-    </row>
-    <row r="11" spans="1:32" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG10" s="2"/>
+      <c r="AH10" s="2"/>
+      <c r="AI10" s="2"/>
+    </row>
+    <row r="11" spans="1:35" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="4"/>
+      <c r="B11" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="C11" s="5">
         <v>44341</v>
       </c>
@@ -924,19 +1036,24 @@
       <c r="W11" s="2"/>
       <c r="X11" s="2"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
+      <c r="Z11" s="18"/>
       <c r="AA11" s="2"/>
       <c r="AB11" s="2"/>
       <c r="AC11" s="2"/>
       <c r="AD11" s="2"/>
       <c r="AE11" s="2"/>
       <c r="AF11" s="2"/>
-    </row>
-    <row r="12" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG11" s="2"/>
+      <c r="AH11" s="2"/>
+      <c r="AI11" s="2"/>
+    </row>
+    <row r="12" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="3"/>
+      <c r="B12" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="C12" s="5">
         <v>44342</v>
       </c>
@@ -965,18 +1082,23 @@
       <c r="X12" s="2"/>
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="2"/>
+      <c r="AA12" s="18"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="18"/>
       <c r="AD12" s="2"/>
       <c r="AE12" s="2"/>
       <c r="AF12" s="2"/>
-    </row>
-    <row r="13" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG12" s="2"/>
+      <c r="AH12" s="2"/>
+      <c r="AI12" s="2"/>
+    </row>
+    <row r="13" spans="1:35" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="3"/>
+      <c r="B13" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="C13" s="5">
         <v>44342</v>
       </c>
@@ -1005,18 +1127,23 @@
       <c r="X13" s="2"/>
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
-      <c r="AA13" s="2"/>
-      <c r="AB13" s="2"/>
-      <c r="AC13" s="2"/>
-      <c r="AD13" s="2"/>
-      <c r="AE13" s="2"/>
+      <c r="AA13" s="18"/>
+      <c r="AB13" s="18"/>
+      <c r="AC13" s="18"/>
+      <c r="AD13" s="18"/>
+      <c r="AE13" s="19"/>
       <c r="AF13" s="2"/>
-    </row>
-    <row r="14" spans="1:32" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AG13" s="2"/>
+      <c r="AH13" s="2"/>
+      <c r="AI13" s="2"/>
+    </row>
+    <row r="14" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B14" s="3"/>
+      <c r="B14" s="9" t="s">
+        <v>15</v>
+      </c>
       <c r="C14" s="5">
         <v>44342</v>
       </c>
@@ -1045,22 +1172,29 @@
       <c r="X14" s="2"/>
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="2"/>
-      <c r="AD14" s="2"/>
-      <c r="AE14" s="2"/>
-      <c r="AF14" s="2"/>
-    </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="AA14" s="18"/>
+      <c r="AB14" s="18"/>
+      <c r="AC14" s="18"/>
+      <c r="AD14" s="18"/>
+      <c r="AE14" s="18"/>
+      <c r="AF14" s="18"/>
+      <c r="AG14" s="2"/>
+      <c r="AH14" s="2"/>
+      <c r="AI14" s="2"/>
+    </row>
+    <row r="15" spans="1:35" ht="36" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="B15" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D15" s="13">
+        <v>44377</v>
+      </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
@@ -1080,23 +1214,32 @@
       <c r="U15" s="2"/>
       <c r="V15" s="2"/>
       <c r="W15" s="2"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="2"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="2"/>
-      <c r="AD15" s="2"/>
-      <c r="AE15" s="2"/>
-      <c r="AF15" s="2"/>
-    </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="X15" s="19"/>
+      <c r="Y15" s="19"/>
+      <c r="Z15" s="19"/>
+      <c r="AA15" s="19"/>
+      <c r="AB15" s="19"/>
+      <c r="AC15" s="19"/>
+      <c r="AD15" s="19"/>
+      <c r="AE15" s="19"/>
+      <c r="AF15" s="19"/>
+      <c r="AG15" s="2"/>
+      <c r="AH15" s="18"/>
+      <c r="AI15" s="18"/>
+    </row>
+    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="B16" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="13">
+        <v>44362</v>
+      </c>
+      <c r="D16" s="13">
+        <v>44362</v>
+      </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
@@ -1108,7 +1251,7 @@
       <c r="M16" s="2"/>
       <c r="N16" s="2"/>
       <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
+      <c r="P16" s="19"/>
       <c r="Q16" s="2"/>
       <c r="R16" s="2"/>
       <c r="S16" s="2"/>
@@ -1116,7 +1259,7 @@
       <c r="U16" s="2"/>
       <c r="V16" s="2"/>
       <c r="W16" s="2"/>
-      <c r="X16" s="2"/>
+      <c r="X16" s="19"/>
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
       <c r="AA16" s="2"/>
@@ -1125,14 +1268,23 @@
       <c r="AD16" s="2"/>
       <c r="AE16" s="2"/>
       <c r="AF16" s="2"/>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="AG16" s="18"/>
+      <c r="AH16" s="2"/>
+      <c r="AI16" s="2"/>
+    </row>
+    <row r="17" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="B17" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D17" s="13">
+        <v>44370</v>
+      </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
@@ -1152,7 +1304,7 @@
       <c r="U17" s="2"/>
       <c r="V17" s="2"/>
       <c r="W17" s="2"/>
-      <c r="X17" s="2"/>
+      <c r="X17" s="19"/>
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
       <c r="AA17" s="2"/>
@@ -1161,14 +1313,23 @@
       <c r="AD17" s="2"/>
       <c r="AE17" s="2"/>
       <c r="AF17" s="2"/>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="AG17" s="2"/>
+      <c r="AH17" s="18"/>
+      <c r="AI17" s="2"/>
+    </row>
+    <row r="18" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="B18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D18" s="13">
+        <v>44370</v>
+      </c>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
@@ -1188,7 +1349,7 @@
       <c r="U18" s="2"/>
       <c r="V18" s="2"/>
       <c r="W18" s="2"/>
-      <c r="X18" s="2"/>
+      <c r="X18" s="19"/>
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
       <c r="AA18" s="2"/>
@@ -1197,14 +1358,23 @@
       <c r="AD18" s="2"/>
       <c r="AE18" s="2"/>
       <c r="AF18" s="2"/>
-    </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
+      <c r="AG18" s="2"/>
+      <c r="AH18" s="18"/>
+      <c r="AI18" s="2"/>
+    </row>
+    <row r="19" spans="1:35" ht="24" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="B19" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D19" s="13">
+        <v>44370</v>
+      </c>
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
@@ -1224,7 +1394,7 @@
       <c r="U19" s="2"/>
       <c r="V19" s="2"/>
       <c r="W19" s="2"/>
-      <c r="X19" s="2"/>
+      <c r="X19" s="19"/>
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
       <c r="AA19" s="2"/>
@@ -1233,46 +1403,281 @@
       <c r="AD19" s="2"/>
       <c r="AE19" s="2"/>
       <c r="AF19" s="2"/>
-    </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+      <c r="AG19" s="2"/>
+      <c r="AH19" s="18"/>
+      <c r="AI19" s="2"/>
+    </row>
+    <row r="20" spans="1:35" ht="36" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="B20" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D20" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="2"/>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+      <c r="O20" s="2"/>
+      <c r="P20" s="2"/>
+      <c r="Q20" s="2"/>
+      <c r="R20" s="2"/>
+      <c r="S20" s="2"/>
+      <c r="T20" s="2"/>
+      <c r="U20" s="2"/>
+      <c r="V20" s="2"/>
+      <c r="W20" s="2"/>
+      <c r="X20" s="19"/>
+      <c r="Y20" s="2"/>
+      <c r="Z20" s="2"/>
+      <c r="AA20" s="2"/>
+      <c r="AB20" s="2"/>
+      <c r="AC20" s="2"/>
+      <c r="AD20" s="2"/>
+      <c r="AE20" s="2"/>
+      <c r="AF20" s="2"/>
+      <c r="AG20" s="2"/>
+      <c r="AH20" s="18"/>
+      <c r="AI20" s="2"/>
+    </row>
+    <row r="21" spans="1:35" ht="24" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="B21" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D21" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="2"/>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+      <c r="O21" s="2"/>
+      <c r="P21" s="2"/>
+      <c r="Q21" s="2"/>
+      <c r="R21" s="2"/>
+      <c r="S21" s="2"/>
+      <c r="T21" s="2"/>
+      <c r="U21" s="2"/>
+      <c r="V21" s="2"/>
+      <c r="W21" s="2"/>
+      <c r="X21" s="19"/>
+      <c r="Y21" s="2"/>
+      <c r="Z21" s="2"/>
+      <c r="AA21" s="2"/>
+      <c r="AB21" s="2"/>
+      <c r="AC21" s="2"/>
+      <c r="AD21" s="2"/>
+      <c r="AE21" s="2"/>
+      <c r="AF21" s="2"/>
+      <c r="AG21" s="2"/>
+      <c r="AH21" s="18"/>
+      <c r="AI21" s="2"/>
+    </row>
+    <row r="22" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+      <c r="B22" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D22" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="2"/>
+      <c r="L22" s="2"/>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+      <c r="O22" s="2"/>
+      <c r="P22" s="2"/>
+      <c r="Q22" s="2"/>
+      <c r="R22" s="2"/>
+      <c r="S22" s="2"/>
+      <c r="T22" s="2"/>
+      <c r="U22" s="2"/>
+      <c r="V22" s="2"/>
+      <c r="W22" s="2"/>
+      <c r="X22" s="19"/>
+      <c r="Y22" s="2"/>
+      <c r="Z22" s="2"/>
+      <c r="AA22" s="2"/>
+      <c r="AB22" s="2"/>
+      <c r="AC22" s="2"/>
+      <c r="AD22" s="2"/>
+      <c r="AE22" s="2"/>
+      <c r="AF22" s="2"/>
+      <c r="AG22" s="2"/>
+      <c r="AH22" s="18"/>
+      <c r="AI22" s="2"/>
+    </row>
+    <row r="23" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+      <c r="B23" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D23" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="2"/>
+      <c r="M23" s="2"/>
+      <c r="N23" s="2"/>
+      <c r="O23" s="2"/>
+      <c r="P23" s="2"/>
+      <c r="Q23" s="2"/>
+      <c r="R23" s="2"/>
+      <c r="S23" s="2"/>
+      <c r="T23" s="2"/>
+      <c r="U23" s="2"/>
+      <c r="V23" s="2"/>
+      <c r="W23" s="2"/>
+      <c r="X23" s="19"/>
+      <c r="Y23" s="2"/>
+      <c r="Z23" s="2"/>
+      <c r="AA23" s="2"/>
+      <c r="AB23" s="2"/>
+      <c r="AC23" s="2"/>
+      <c r="AD23" s="2"/>
+      <c r="AE23" s="2"/>
+      <c r="AF23" s="2"/>
+      <c r="AG23" s="2"/>
+      <c r="AH23" s="18"/>
+      <c r="AI23" s="2"/>
+    </row>
+    <row r="24" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
+      <c r="B24" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D24" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="2"/>
+      <c r="L24" s="2"/>
+      <c r="M24" s="2"/>
+      <c r="N24" s="2"/>
+      <c r="O24" s="2"/>
+      <c r="P24" s="2"/>
+      <c r="Q24" s="2"/>
+      <c r="R24" s="2"/>
+      <c r="S24" s="2"/>
+      <c r="T24" s="2"/>
+      <c r="U24" s="2"/>
+      <c r="V24" s="2"/>
+      <c r="W24" s="2"/>
+      <c r="X24" s="19"/>
+      <c r="Y24" s="2"/>
+      <c r="Z24" s="2"/>
+      <c r="AA24" s="2"/>
+      <c r="AB24" s="2"/>
+      <c r="AC24" s="2"/>
+      <c r="AD24" s="2"/>
+      <c r="AE24" s="2"/>
+      <c r="AF24" s="2"/>
+      <c r="AG24" s="2"/>
+      <c r="AH24" s="18"/>
+      <c r="AI24" s="2"/>
+    </row>
+    <row r="25" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="B25" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25" s="13">
+        <v>44370</v>
+      </c>
+      <c r="D25" s="13">
+        <v>44370</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
+      <c r="H25" s="2"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="2"/>
+      <c r="M25" s="2"/>
+      <c r="N25" s="2"/>
+      <c r="O25" s="2"/>
+      <c r="P25" s="2"/>
+      <c r="Q25" s="2"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="2"/>
+      <c r="T25" s="2"/>
+      <c r="U25" s="2"/>
+      <c r="V25" s="2"/>
+      <c r="W25" s="2"/>
+      <c r="X25" s="19"/>
+      <c r="Y25" s="2"/>
+      <c r="Z25" s="2"/>
+      <c r="AA25" s="2"/>
+      <c r="AB25" s="2"/>
+      <c r="AC25" s="2"/>
+      <c r="AD25" s="2"/>
+      <c r="AE25" s="2"/>
+      <c r="AF25" s="2"/>
+      <c r="AG25" s="2"/>
+      <c r="AH25" s="18"/>
+      <c r="AI25" s="2"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E9:AF14">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND($C9&lt;=E$4,$D9&gt;=E$4)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="0" priority="3">
-      <formula>AND($C9&lt;=E$4,$D9&gt;=E$4)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>